<commit_message>
feat: Enhance extract_kunden_to_excel.py with env var input, profile system, and timestamped output
This commit includes the following enhancements to the extract_kunden_to_excel.py script:

- Replaced argument parsing with an environment variable (KUNDEN_INPUT_DIR) for specifying the input directory.
- Implemented a profile system to handle different extraction profiles (details to be implemented in a future commit).
- Changed the output file name to kgs{timestamp}.xlsx, where timestamp is the current date and time in the format YYYYMMDD_HHMMSS.
</commit_message>
<xml_diff>
--- a/kgs_001_ER70_p_20250616.xlsx
+++ b/kgs_001_ER70_p_20250616.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmiliosRichards\Projects\Company Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D48A2F0-AAFC-4B38-B56C-CC271379FAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612D1BD-3B4C-46B1-B36C-11C6058F134D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1096">
   <si>
     <t>Company Name</t>
   </si>
@@ -3172,12 +3172,180 @@
   <si>
     <t>Avg Leads Per Day</t>
   </si>
+  <si>
+    <t>Targets_Specific_Industry_Type</t>
+  </si>
+  <si>
+    <t>Is_Startup</t>
+  </si>
+  <si>
+    <t>Is_AI_Software</t>
+  </si>
+  <si>
+    <t>Is_Innovative_Product</t>
+  </si>
+  <si>
+    <t>Is_Disruptive_Product</t>
+  </si>
+  <si>
+    <t>Is_VC_Funded</t>
+  </si>
+  <si>
+    <t>Is_SaaS_Software</t>
+  </si>
+  <si>
+    <t>Is_Complex_Solution</t>
+  </si>
+  <si>
+    <t>Is_Investment_Product</t>
+  </si>
+  <si>
+    <t>Partner_Targets_B2B</t>
+  </si>
+  <si>
+    <t>Partner_Target_Audience_Size_Over_1000</t>
+  </si>
+  <si>
+    <t>Manufacturing (General); Manufacturing (Chemicals/Pharma Production); B2B (General)</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities)</t>
+  </si>
+  <si>
+    <t>SMEs (General B2B - targeting small to medium businesses across various industries); Public Sector / Government; Manufacturing (Automotive)</t>
+  </si>
+  <si>
+    <t>HR / Recruitment Services; Healthcare (General/Other); Consulting (General Business/Management - if not fitting a more specific tech/industry consulting)</t>
+  </si>
+  <si>
+    <t>SMEs (General B2B - targeting small to medium businesses across various industries); Large Enterprises (General B2B - targeting large corporations across various industries); Manufacturing (General)</t>
+  </si>
+  <si>
+    <t>B2B (General - use if no specific industry is clear but it's clearly B2B)</t>
+  </si>
+  <si>
+    <t>Logistics &amp; Supply Chain Sector</t>
+  </si>
+  <si>
+    <t>SMEs (General B2B - targeting small to medium businesses across various industries); Large Enterprises (General B2B - targeting large corporations across various industries)</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities); Healthcare (General/Other)</t>
+  </si>
+  <si>
+    <t>Healthcare (Hospitals/Clinics)</t>
+  </si>
+  <si>
+    <t>Aerospace / Aviation Sector; EdTech / E-Learning Providers; Software Development / Tech Companies (B2B)</t>
+  </si>
+  <si>
+    <t>Healthcare (General/Other); Software Development / Tech Companies (B2B)</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities); Healthcare (Hospitals/Clinics); Healthcare (General/Other)</t>
+  </si>
+  <si>
+    <t>SMEs (General B2B - targeting small to medium businesses across various industries)</t>
+  </si>
+  <si>
+    <t>IT Services / Managed Services; Software Development / Tech Companies (B2B); B2B (General)</t>
+  </si>
+  <si>
+    <t>Logistics &amp; Supply Chain Sector; Manufacturing (General); Large Enterprises (General B2B)</t>
+  </si>
+  <si>
+    <t>IT Services / Managed Services; Cybersecurity Services; B2B (General - use if no specific industry is clear but it's clearly B2B)</t>
+  </si>
+  <si>
+    <t>IT Services / Managed Services; Large Enterprises (General B2B - targeting large corporations across various industries)</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities); Healthcare (Hospitals/Clinics); B2B (General)</t>
+  </si>
+  <si>
+    <t>Legal Sector</t>
+  </si>
+  <si>
+    <t>Energy Sector (incl. Renewables); Food &amp; Beverage (Producers/Services)</t>
+  </si>
+  <si>
+    <t>Healthcare (Hospitals/Clinics); Healthcare (Care Facilities)</t>
+  </si>
+  <si>
+    <t>Consulting (General Business/Management - if not fitting a more specific tech/industry consulting)</t>
+  </si>
+  <si>
+    <t>Tax / Accounting Sector; Aerospace / Aviation Sector</t>
+  </si>
+  <si>
+    <t>Healthcare (Hospitals/Clinics); Healthcare (General/Other)</t>
+  </si>
+  <si>
+    <t>Legal Sector; Tax / Accounting Sector</t>
+  </si>
+  <si>
+    <t>Tax / Accounting Sector</t>
+  </si>
+  <si>
+    <t>B2B (General); Media / Publishing / Entertainment; Retail (E-commerce)</t>
+  </si>
+  <si>
+    <t>Hospitality (Hotels, Restaurants, Travel); B2B (General)</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Tax / Accounting Sector; SMEs (General B2B - targeting small to medium businesses across various industries)</t>
+  </si>
+  <si>
+    <t>Other Specific Niche B2B; Real Estate / Construction Sector</t>
+  </si>
+  <si>
+    <t>Legal Sector; Tax / Accounting Sector; Financial Services (Investment/Wealth Management)</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage (Producers/Services); Manufacturing (Chemicals/Pharma Production); Logistics &amp; Supply Chain Sector</t>
+  </si>
+  <si>
+    <t>Retail (E-commerce); Logistics &amp; Supply Chain Sector; Large Enterprises (General B2B)</t>
+  </si>
+  <si>
+    <t>Manufacturing (General); B2B (General)</t>
+  </si>
+  <si>
+    <t>Healthcare (General/Other)</t>
+  </si>
+  <si>
+    <t>Real Estate / Construction Sector</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities); Healthcare (Hospitals/Clinics)</t>
+  </si>
+  <si>
+    <t>Real Estate / Construction Sector; Manufacturing (General); Retail (Brick &amp; Mortar)</t>
+  </si>
+  <si>
+    <t>SMEs (General B2B - targeting small to medium businesses across various industries); Real Estate / Construction Sector; Manufacturing (General)</t>
+  </si>
+  <si>
+    <t>Manufacturing (Machinery/Industrial); Energy Sector (incl. Renewables); Manufacturing (General)</t>
+  </si>
+  <si>
+    <t>Healthcare (Care Facilities); IT Services / Managed Services</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3210,6 +3378,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3293,21 +3476,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3391,9 +3581,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="KundenTable" displayName="KundenTable" ref="A1:U71">
-  <autoFilter ref="A1:U71" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="KundenTable" displayName="KundenTable" ref="A1:AF71">
+  <autoFilter ref="A1:AF71" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="32">
     <tableColumn id="21" xr3:uid="{9932E1E9-CEDD-4612-8EC6-984F64B5C7C8}" name="Avg Leads Per Day" dataDxfId="1"/>
     <tableColumn id="23" xr3:uid="{27104F3D-FFD2-4B58-9245-3A530A37C0D6}" name="Evaluation Score" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Company Name"/>
@@ -3415,6 +3605,17 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Phone"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Source Document Section/Notes"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Is Successful Partner"/>
+    <tableColumn id="31" xr3:uid="{13467E8D-EBF5-42E3-879F-911F5638B3C6}" name="Partner_Targets_B2B"/>
+    <tableColumn id="32" xr3:uid="{5178E0BC-1878-4659-AF89-7B4D4F0ABBE7}" name="Partner_Target_Audience_Size_Over_1000"/>
+    <tableColumn id="18" xr3:uid="{CE72D566-D3CA-407C-8E9A-05C6FC3FBE99}" name="Targets_Specific_Industry_Type"/>
+    <tableColumn id="19" xr3:uid="{841498E3-98D5-4914-9C31-CB82EF66C5F5}" name="Is_Startup"/>
+    <tableColumn id="24" xr3:uid="{8CAA6712-B8F6-4055-BABB-3CDFC72A7AE4}" name="Is_AI_Software"/>
+    <tableColumn id="25" xr3:uid="{E1A2F166-6F87-41AB-AB55-B39B32CC11FC}" name="Is_Innovative_Product"/>
+    <tableColumn id="26" xr3:uid="{F16A620D-F21A-4E73-AC1A-2C5C57C099A8}" name="Is_Disruptive_Product"/>
+    <tableColumn id="27" xr3:uid="{89E6EAA9-49F1-42A8-984C-3FEBE1D48DCB}" name="Is_VC_Funded"/>
+    <tableColumn id="28" xr3:uid="{9ACF214A-008C-48FD-8B22-0751BFB9F443}" name="Is_SaaS_Software"/>
+    <tableColumn id="29" xr3:uid="{0A17F917-52DA-4EB7-92FF-6A7608A4AEF9}" name="Is_Complex_Solution"/>
+    <tableColumn id="30" xr3:uid="{2302B6AF-B421-44F7-B8FA-51FE031319EF}" name="Is_Investment_Product"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3705,10 +3906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:AF71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,9 +3922,9 @@
     <col min="6" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="124.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="232.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="56" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="208.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="159.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30.28515625" bestFit="1" customWidth="1"/>
@@ -3731,11 +3932,21 @@
     <col min="18" max="18" width="37" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="35" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="44" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="191" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1039</v>
       </c>
@@ -3799,8 +4010,41 @@
       <c r="U1" s="1" t="s">
         <v>973</v>
       </c>
+      <c r="V1" s="10" t="s">
+        <v>1049</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>1047</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>1048</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
@@ -3860,8 +4104,41 @@
       <c r="U2" t="s">
         <v>26</v>
       </c>
+      <c r="V2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="9"/>
       <c r="C3" t="s">
@@ -3915,8 +4192,41 @@
       <c r="U3" t="s">
         <v>26</v>
       </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="8"/>
       <c r="C4" t="s">
@@ -3973,8 +4283,41 @@
       <c r="U4" t="s">
         <v>26</v>
       </c>
+      <c r="V4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="9"/>
       <c r="C5" t="s">
@@ -4031,8 +4374,41 @@
       <c r="U5" t="s">
         <v>26</v>
       </c>
+      <c r="V5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
@@ -4086,8 +4462,41 @@
       <c r="U6" t="s">
         <v>26</v>
       </c>
+      <c r="V6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="9"/>
       <c r="C7" t="s">
@@ -4147,8 +4556,41 @@
       <c r="U7" t="s">
         <v>26</v>
       </c>
+      <c r="V7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="8"/>
       <c r="C8" t="s">
@@ -4205,8 +4647,41 @@
       <c r="U8" t="s">
         <v>26</v>
       </c>
+      <c r="V8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="9"/>
       <c r="C9" t="s">
@@ -4266,8 +4741,41 @@
       <c r="U9" t="s">
         <v>26</v>
       </c>
+      <c r="V9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="8"/>
       <c r="C10" t="s">
@@ -4321,8 +4829,41 @@
       <c r="U10" t="s">
         <v>26</v>
       </c>
+      <c r="V10" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="9"/>
       <c r="C11" t="s">
@@ -4382,8 +4923,41 @@
       <c r="U11" t="s">
         <v>26</v>
       </c>
+      <c r="V11" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11" t="s">
+        <v>26</v>
+      </c>
+      <c r="X11" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="8"/>
       <c r="C12" t="s">
@@ -4440,8 +5014,41 @@
       <c r="U12" t="s">
         <v>26</v>
       </c>
+      <c r="V12" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="9"/>
       <c r="C13" t="s">
@@ -4501,8 +5108,41 @@
       <c r="U13" t="s">
         <v>26</v>
       </c>
+      <c r="V13" t="s">
+        <v>26</v>
+      </c>
+      <c r="W13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="8"/>
       <c r="C14" t="s">
@@ -4562,8 +5202,41 @@
       <c r="U14" t="s">
         <v>26</v>
       </c>
+      <c r="V14" t="s">
+        <v>26</v>
+      </c>
+      <c r="W14" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="9"/>
       <c r="C15" t="s">
@@ -4623,8 +5296,41 @@
       <c r="U15" t="s">
         <v>26</v>
       </c>
+      <c r="V15" t="s">
+        <v>26</v>
+      </c>
+      <c r="W15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" t="s">
+        <v>1062</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
@@ -4684,8 +5390,41 @@
       <c r="U16" t="s">
         <v>26</v>
       </c>
+      <c r="V16" t="s">
+        <v>26</v>
+      </c>
+      <c r="W16" t="s">
+        <v>26</v>
+      </c>
+      <c r="X16" t="s">
+        <v>1063</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="9"/>
       <c r="C17" t="s">
@@ -4745,8 +5484,41 @@
       <c r="U17" t="s">
         <v>26</v>
       </c>
+      <c r="V17" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" t="s">
+        <v>26</v>
+      </c>
+      <c r="X17" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="8"/>
       <c r="C18" t="s">
@@ -4806,8 +5578,41 @@
       <c r="U18" t="s">
         <v>26</v>
       </c>
+      <c r="V18" t="s">
+        <v>26</v>
+      </c>
+      <c r="W18" t="s">
+        <v>26</v>
+      </c>
+      <c r="X18" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="9"/>
       <c r="C19" t="s">
@@ -4867,8 +5672,41 @@
       <c r="U19" t="s">
         <v>26</v>
       </c>
+      <c r="V19" t="s">
+        <v>26</v>
+      </c>
+      <c r="W19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X19" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="8"/>
       <c r="C20" t="s">
@@ -4928,8 +5766,41 @@
       <c r="U20" t="s">
         <v>26</v>
       </c>
+      <c r="V20" t="s">
+        <v>26</v>
+      </c>
+      <c r="W20" t="s">
+        <v>26</v>
+      </c>
+      <c r="X20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="9"/>
       <c r="C21" t="s">
@@ -4989,8 +5860,41 @@
       <c r="U21" t="s">
         <v>26</v>
       </c>
+      <c r="V21" t="s">
+        <v>26</v>
+      </c>
+      <c r="W21" t="s">
+        <v>26</v>
+      </c>
+      <c r="X21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="8"/>
       <c r="C22" t="s">
@@ -5050,8 +5954,41 @@
       <c r="U22" t="s">
         <v>26</v>
       </c>
+      <c r="V22" t="s">
+        <v>26</v>
+      </c>
+      <c r="W22" t="s">
+        <v>26</v>
+      </c>
+      <c r="X22" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9"/>
       <c r="C23" t="s">
@@ -5111,8 +6048,41 @@
       <c r="U23" t="s">
         <v>26</v>
       </c>
+      <c r="V23" t="s">
+        <v>26</v>
+      </c>
+      <c r="W23" t="s">
+        <v>26</v>
+      </c>
+      <c r="X23" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="8"/>
       <c r="C24" t="s">
@@ -5166,8 +6136,41 @@
       <c r="U24" t="s">
         <v>26</v>
       </c>
+      <c r="V24" t="s">
+        <v>26</v>
+      </c>
+      <c r="W24" t="s">
+        <v>26</v>
+      </c>
+      <c r="X24" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="9"/>
       <c r="C25" t="s">
@@ -5224,8 +6227,41 @@
       <c r="U25" t="s">
         <v>26</v>
       </c>
+      <c r="V25" t="s">
+        <v>26</v>
+      </c>
+      <c r="W25" t="s">
+        <v>26</v>
+      </c>
+      <c r="X25" t="s">
+        <v>1068</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="8"/>
       <c r="C26" t="s">
@@ -5285,8 +6321,41 @@
       <c r="U26" t="s">
         <v>26</v>
       </c>
+      <c r="V26" t="s">
+        <v>26</v>
+      </c>
+      <c r="W26" t="s">
+        <v>26</v>
+      </c>
+      <c r="X26" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="9"/>
       <c r="C27" t="s">
@@ -5346,8 +6415,41 @@
       <c r="U27" t="s">
         <v>26</v>
       </c>
+      <c r="V27" t="s">
+        <v>26</v>
+      </c>
+      <c r="W27" t="s">
+        <v>26</v>
+      </c>
+      <c r="X27" t="s">
+        <v>1052</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="8"/>
       <c r="C28" t="s">
@@ -5401,8 +6503,41 @@
       <c r="U28" t="s">
         <v>26</v>
       </c>
+      <c r="V28" t="s">
+        <v>26</v>
+      </c>
+      <c r="W28" t="s">
+        <v>26</v>
+      </c>
+      <c r="X28" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="9"/>
       <c r="C29" t="s">
@@ -5462,8 +6597,41 @@
       <c r="U29" t="s">
         <v>26</v>
       </c>
+      <c r="V29" t="s">
+        <v>26</v>
+      </c>
+      <c r="W29" t="s">
+        <v>26</v>
+      </c>
+      <c r="X29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="8"/>
       <c r="C30" t="s">
@@ -5523,8 +6691,41 @@
       <c r="U30" t="s">
         <v>26</v>
       </c>
+      <c r="V30" t="s">
+        <v>26</v>
+      </c>
+      <c r="W30" t="s">
+        <v>26</v>
+      </c>
+      <c r="X30" t="s">
+        <v>1072</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="9"/>
       <c r="C31" t="s">
@@ -5584,8 +6785,41 @@
       <c r="U31" t="s">
         <v>26</v>
       </c>
+      <c r="V31" t="s">
+        <v>26</v>
+      </c>
+      <c r="W31" t="s">
+        <v>26</v>
+      </c>
+      <c r="X31" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
@@ -5645,8 +6879,41 @@
       <c r="U32" t="s">
         <v>26</v>
       </c>
+      <c r="V32" t="s">
+        <v>26</v>
+      </c>
+      <c r="W32" t="s">
+        <v>26</v>
+      </c>
+      <c r="X32" t="s">
+        <v>1074</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="9"/>
       <c r="C33" t="s">
@@ -5703,8 +6970,41 @@
       <c r="U33" t="s">
         <v>26</v>
       </c>
+      <c r="V33" t="s">
+        <v>26</v>
+      </c>
+      <c r="W33" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" t="s">
+        <v>1052</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="8"/>
       <c r="C34" t="s">
@@ -5758,8 +7058,41 @@
       <c r="U34" t="s">
         <v>26</v>
       </c>
+      <c r="V34" t="s">
+        <v>26</v>
+      </c>
+      <c r="W34" t="s">
+        <v>26</v>
+      </c>
+      <c r="X34" t="s">
+        <v>1063</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="9"/>
       <c r="C35" t="s">
@@ -5813,8 +7146,41 @@
       <c r="U35" t="s">
         <v>26</v>
       </c>
+      <c r="V35" t="s">
+        <v>26</v>
+      </c>
+      <c r="W35" t="s">
+        <v>26</v>
+      </c>
+      <c r="X35" t="s">
+        <v>1075</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="8"/>
       <c r="C36" t="s">
@@ -5865,8 +7231,41 @@
       <c r="U36" t="s">
         <v>26</v>
       </c>
+      <c r="V36" t="s">
+        <v>26</v>
+      </c>
+      <c r="W36" t="s">
+        <v>26</v>
+      </c>
+      <c r="X36" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="9"/>
       <c r="C37" t="s">
@@ -5920,8 +7319,41 @@
       <c r="U37" t="s">
         <v>26</v>
       </c>
+      <c r="V37" t="s">
+        <v>26</v>
+      </c>
+      <c r="W37" t="s">
+        <v>26</v>
+      </c>
+      <c r="X37" t="s">
+        <v>1076</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="8"/>
       <c r="C38" t="s">
@@ -5975,8 +7407,41 @@
       <c r="U38" t="s">
         <v>26</v>
       </c>
+      <c r="V38" t="s">
+        <v>26</v>
+      </c>
+      <c r="W38" t="s">
+        <v>26</v>
+      </c>
+      <c r="X38" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="9"/>
       <c r="C39" t="s">
@@ -6030,8 +7495,41 @@
       <c r="U39" t="s">
         <v>26</v>
       </c>
+      <c r="V39" t="s">
+        <v>26</v>
+      </c>
+      <c r="W39" t="s">
+        <v>26</v>
+      </c>
+      <c r="X39" t="s">
+        <v>1078</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="8"/>
       <c r="C40" t="s">
@@ -6085,8 +7583,41 @@
       <c r="U40" t="s">
         <v>26</v>
       </c>
+      <c r="V40" t="s">
+        <v>26</v>
+      </c>
+      <c r="W40" t="s">
+        <v>26</v>
+      </c>
+      <c r="X40" t="s">
+        <v>1079</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="9"/>
       <c r="C41" t="s">
@@ -6140,8 +7671,41 @@
       <c r="U41" t="s">
         <v>26</v>
       </c>
+      <c r="V41" t="s">
+        <v>26</v>
+      </c>
+      <c r="W41" t="s">
+        <v>26</v>
+      </c>
+      <c r="X41" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="8"/>
       <c r="C42" t="s">
@@ -6198,8 +7762,41 @@
       <c r="U42" t="s">
         <v>26</v>
       </c>
+      <c r="V42" t="s">
+        <v>26</v>
+      </c>
+      <c r="W42" t="s">
+        <v>26</v>
+      </c>
+      <c r="X42" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="9"/>
       <c r="C43" t="s">
@@ -6256,8 +7853,41 @@
       <c r="U43" t="s">
         <v>26</v>
       </c>
+      <c r="V43" t="s">
+        <v>26</v>
+      </c>
+      <c r="W43" t="s">
+        <v>26</v>
+      </c>
+      <c r="X43" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="8"/>
       <c r="C44" t="s">
@@ -6314,8 +7944,41 @@
       <c r="U44" t="s">
         <v>26</v>
       </c>
+      <c r="V44" t="s">
+        <v>26</v>
+      </c>
+      <c r="W44" t="s">
+        <v>26</v>
+      </c>
+      <c r="X44" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="9"/>
       <c r="C45" t="s">
@@ -6369,8 +8032,41 @@
       <c r="U45" t="s">
         <v>26</v>
       </c>
+      <c r="V45" t="s">
+        <v>26</v>
+      </c>
+      <c r="W45" t="s">
+        <v>26</v>
+      </c>
+      <c r="X45" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="8"/>
       <c r="C46" t="s">
@@ -6430,8 +8126,41 @@
       <c r="U46" t="s">
         <v>26</v>
       </c>
+      <c r="V46" t="s">
+        <v>26</v>
+      </c>
+      <c r="W46" t="s">
+        <v>26</v>
+      </c>
+      <c r="X46" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="9"/>
       <c r="C47" t="s">
@@ -6491,8 +8220,41 @@
       <c r="U47" t="s">
         <v>26</v>
       </c>
+      <c r="V47" t="s">
+        <v>26</v>
+      </c>
+      <c r="W47" t="s">
+        <v>26</v>
+      </c>
+      <c r="X47" t="s">
+        <v>981</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="8"/>
       <c r="C48" t="s">
@@ -6552,8 +8314,41 @@
       <c r="U48" t="s">
         <v>26</v>
       </c>
+      <c r="V48" t="s">
+        <v>26</v>
+      </c>
+      <c r="W48" t="s">
+        <v>26</v>
+      </c>
+      <c r="X48" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="9"/>
       <c r="C49" t="s">
@@ -6613,8 +8408,41 @@
       <c r="U49" t="s">
         <v>26</v>
       </c>
+      <c r="V49" t="s">
+        <v>26</v>
+      </c>
+      <c r="W49" t="s">
+        <v>26</v>
+      </c>
+      <c r="X49" t="s">
+        <v>1081</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="8"/>
       <c r="C50" t="s">
@@ -6674,8 +8502,41 @@
       <c r="U50" t="s">
         <v>26</v>
       </c>
+      <c r="V50" t="s">
+        <v>26</v>
+      </c>
+      <c r="W50" t="s">
+        <v>26</v>
+      </c>
+      <c r="X50" t="s">
+        <v>1082</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="9"/>
       <c r="C51" t="s">
@@ -6732,8 +8593,41 @@
       <c r="U51" t="s">
         <v>26</v>
       </c>
+      <c r="V51" t="s">
+        <v>26</v>
+      </c>
+      <c r="W51" t="s">
+        <v>26</v>
+      </c>
+      <c r="X51" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="8"/>
       <c r="C52" t="s">
@@ -6793,8 +8687,41 @@
       <c r="U52" t="s">
         <v>26</v>
       </c>
+      <c r="V52" t="s">
+        <v>26</v>
+      </c>
+      <c r="W52" t="s">
+        <v>26</v>
+      </c>
+      <c r="X52" t="s">
+        <v>1084</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="9"/>
       <c r="C53" t="s">
@@ -6848,8 +8775,41 @@
       <c r="U53" t="s">
         <v>26</v>
       </c>
+      <c r="V53" t="s">
+        <v>26</v>
+      </c>
+      <c r="W53" t="s">
+        <v>26</v>
+      </c>
+      <c r="X53" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="8"/>
       <c r="C54" t="s">
@@ -6906,8 +8866,41 @@
       <c r="U54" t="s">
         <v>26</v>
       </c>
+      <c r="V54" t="s">
+        <v>26</v>
+      </c>
+      <c r="W54" t="s">
+        <v>26</v>
+      </c>
+      <c r="X54" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="9"/>
       <c r="C55" t="s">
@@ -6967,8 +8960,41 @@
       <c r="U55" t="s">
         <v>26</v>
       </c>
+      <c r="V55" t="s">
+        <v>26</v>
+      </c>
+      <c r="W55" t="s">
+        <v>26</v>
+      </c>
+      <c r="X55" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="8"/>
       <c r="C56" t="s">
@@ -7022,8 +9048,41 @@
       <c r="U56" t="s">
         <v>26</v>
       </c>
+      <c r="V56" t="s">
+        <v>26</v>
+      </c>
+      <c r="W56" t="s">
+        <v>26</v>
+      </c>
+      <c r="X56" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="9"/>
       <c r="C57" t="s">
@@ -7077,8 +9136,41 @@
       <c r="U57" t="s">
         <v>26</v>
       </c>
+      <c r="V57" t="s">
+        <v>26</v>
+      </c>
+      <c r="W57" t="s">
+        <v>26</v>
+      </c>
+      <c r="X57" t="s">
+        <v>1086</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="8"/>
       <c r="C58" t="s">
@@ -7132,8 +9224,41 @@
       <c r="U58" t="s">
         <v>26</v>
       </c>
+      <c r="V58" t="s">
+        <v>26</v>
+      </c>
+      <c r="W58" t="s">
+        <v>26</v>
+      </c>
+      <c r="X58" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="9"/>
       <c r="C59" t="s">
@@ -7193,8 +9318,41 @@
       <c r="U59" t="s">
         <v>26</v>
       </c>
+      <c r="V59" t="s">
+        <v>26</v>
+      </c>
+      <c r="W59" t="s">
+        <v>26</v>
+      </c>
+      <c r="X59" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="8"/>
       <c r="C60" t="s">
@@ -7248,8 +9406,41 @@
       <c r="U60" t="s">
         <v>26</v>
       </c>
+      <c r="V60" t="s">
+        <v>26</v>
+      </c>
+      <c r="W60" t="s">
+        <v>26</v>
+      </c>
+      <c r="X60" t="s">
+        <v>1081</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="9"/>
       <c r="C61" t="s">
@@ -7309,8 +9500,41 @@
       <c r="U61" t="s">
         <v>26</v>
       </c>
+      <c r="V61" t="s">
+        <v>26</v>
+      </c>
+      <c r="W61" t="s">
+        <v>26</v>
+      </c>
+      <c r="X61" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="8"/>
       <c r="C62" t="s">
@@ -7364,8 +9588,41 @@
       <c r="U62" t="s">
         <v>26</v>
       </c>
+      <c r="V62" t="s">
+        <v>26</v>
+      </c>
+      <c r="W62" t="s">
+        <v>26</v>
+      </c>
+      <c r="X62" t="s">
+        <v>1052</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF62" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="9"/>
       <c r="C63" t="s">
@@ -7416,8 +9673,41 @@
       <c r="U63" t="s">
         <v>26</v>
       </c>
+      <c r="V63" t="s">
+        <v>26</v>
+      </c>
+      <c r="W63" t="s">
+        <v>26</v>
+      </c>
+      <c r="X63" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="8"/>
       <c r="C64" t="s">
@@ -7474,8 +9764,41 @@
       <c r="U64" t="s">
         <v>26</v>
       </c>
+      <c r="V64" t="s">
+        <v>26</v>
+      </c>
+      <c r="W64" t="s">
+        <v>26</v>
+      </c>
+      <c r="X64" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="9"/>
       <c r="C65" t="s">
@@ -7532,8 +9855,41 @@
       <c r="U65" t="s">
         <v>26</v>
       </c>
+      <c r="V65" t="s">
+        <v>26</v>
+      </c>
+      <c r="W65" t="s">
+        <v>26</v>
+      </c>
+      <c r="X65" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="8"/>
       <c r="C66" t="s">
@@ -7593,8 +9949,41 @@
       <c r="U66" t="s">
         <v>26</v>
       </c>
+      <c r="V66" t="s">
+        <v>26</v>
+      </c>
+      <c r="W66" t="s">
+        <v>26</v>
+      </c>
+      <c r="X66" t="s">
+        <v>1090</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="9"/>
       <c r="C67" t="s">
@@ -7654,8 +10043,41 @@
       <c r="U67" t="s">
         <v>26</v>
       </c>
+      <c r="V67" t="s">
+        <v>26</v>
+      </c>
+      <c r="W67" t="s">
+        <v>26</v>
+      </c>
+      <c r="X67" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="8"/>
       <c r="C68" t="s">
@@ -7709,8 +10131,41 @@
       <c r="U68" t="s">
         <v>26</v>
       </c>
+      <c r="V68" t="s">
+        <v>26</v>
+      </c>
+      <c r="W68" t="s">
+        <v>26</v>
+      </c>
+      <c r="X68" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="9"/>
       <c r="C69" t="s">
@@ -7770,8 +10225,41 @@
       <c r="U69" t="s">
         <v>26</v>
       </c>
+      <c r="V69" t="s">
+        <v>26</v>
+      </c>
+      <c r="W69" t="s">
+        <v>26</v>
+      </c>
+      <c r="X69" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="8"/>
       <c r="C70" t="s">
@@ -7831,8 +10319,41 @@
       <c r="U70" t="s">
         <v>26</v>
       </c>
+      <c r="V70" t="s">
+        <v>26</v>
+      </c>
+      <c r="W70" t="s">
+        <v>26</v>
+      </c>
+      <c r="X70" t="s">
+        <v>1093</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="9"/>
       <c r="C71" t="s">
@@ -7883,12 +10404,46 @@
       <c r="U71" t="s">
         <v>26</v>
       </c>
+      <c r="V71" t="s">
+        <v>26</v>
+      </c>
+      <c r="W71" t="s">
+        <v>26</v>
+      </c>
+      <c r="X71" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>1095</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>